<commit_message>
[Bug] Fixed skipping of single part sets
</commit_message>
<xml_diff>
--- a/R-package/data/test-data/standard/ODM_dictionary_9.9.9.xlsx
+++ b/R-package/data/test-data/standard/ODM_dictionary_9.9.9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rostylavvyuha/Documents/R work/PHES-ODM/PHES-ODM/R-package/data/test-data/standard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C061EA21-8D1D-654D-BB41-A17896317902}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDC83F5-AB59-3F40-8EDB-21DE47C4F359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="77">
   <si>
     <t>label</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>Excel_part_pass</t>
+  </si>
+  <si>
+    <t>some data</t>
   </si>
 </sst>
 </file>
@@ -784,10 +787,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29077EA8-B5D5-FC4B-9C95-48BEB02322E3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1347,7 +1356,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1359,7 +1374,13 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1368,10 +1389,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FBDB2A0-69E1-DC45-AFC1-E8642273F01F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A1" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[Refactor] Added additional failing files to test
</commit_message>
<xml_diff>
--- a/R-package/data/test-data/standard/ODM_dictionary_9.9.9.xlsx
+++ b/R-package/data/test-data/standard/ODM_dictionary_9.9.9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rostylavvyuha/Documents/R work/PHES-ODM/PHES-ODM/R-package/data/test-data/standard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDC83F5-AB59-3F40-8EDB-21DE47C4F359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5200A40-9A8E-264F-BF47-C1DF0B5BF90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="90">
   <si>
     <t>label</t>
   </si>
@@ -258,6 +258,45 @@
   </si>
   <si>
     <t>some data</t>
+  </si>
+  <si>
+    <t>NoSheetForSetPart</t>
+  </si>
+  <si>
+    <t>Should Fail</t>
+  </si>
+  <si>
+    <t>ShouldFailNoSheetInSet</t>
+  </si>
+  <si>
+    <t>fail/</t>
+  </si>
+  <si>
+    <t>setInSetsFail</t>
+  </si>
+  <si>
+    <t>testing warning</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>hasNoSheet</t>
+  </si>
+  <si>
+    <t>test part for fail</t>
+  </si>
+  <si>
+    <t>NoPartInfoForSet</t>
+  </si>
+  <si>
+    <t>ShouldFailNoPartInfoInSet</t>
+  </si>
+  <si>
+    <t>setInSetsFailWithSheet</t>
+  </si>
+  <si>
+    <t>hasNoPartInfo</t>
   </si>
 </sst>
 </file>
@@ -413,7 +452,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -436,6 +475,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,10 +694,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -776,6 +816,64 @@
       </c>
       <c r="I4" s="14" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -787,7 +885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29077EA8-B5D5-FC4B-9C95-48BEB02322E3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
@@ -803,10 +901,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FBE7DC-C421-DE4D-9F2F-186B46379DBF}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -914,6 +1012,40 @@
       </c>
       <c r="E6" s="14" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A8" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1220,10 +1352,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1341,6 +1473,64 @@
         <v>29</v>
       </c>
       <c r="I4" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="I6" s="18" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Bug] Fixed addHeader not working with varying column counts
</commit_message>
<xml_diff>
--- a/R-package/data/test-data/standard/ODM_dictionary_9.9.9.xlsx
+++ b/R-package/data/test-data/standard/ODM_dictionary_9.9.9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rostylavvyuha/Documents/R work/PHES-ODM/PHES-ODM/R-package/data/test-data/standard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5200A40-9A8E-264F-BF47-C1DF0B5BF90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FA313F-ECF6-BD46-9FA3-82CBCF00A8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="files" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="91">
   <si>
     <t>label</t>
   </si>
@@ -297,6 +297,9 @@
   </si>
   <si>
     <t>hasNoPartInfo</t>
+  </si>
+  <si>
+    <t>something;somethingElse</t>
   </si>
 </sst>
 </file>
@@ -452,7 +455,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -475,7 +478,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -694,10 +696,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -748,7 +750,7 @@
         <v>59</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>11</v>
@@ -875,6 +877,17 @@
       <c r="I6" s="14" t="s">
         <v>80</v>
       </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -903,7 +916,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02FBE7DC-C421-DE4D-9F2F-186B46379DBF}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1530,7 +1543,7 @@
       <c r="H6" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="I6" s="2" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>